<commit_message>
changed client excel file
</commit_message>
<xml_diff>
--- a/src/main/java/com/team5/template/client.xlsx
+++ b/src/main/java/com/team5/template/client.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="63">
   <si>
     <t>Yes</t>
   </si>
@@ -53,9 +53,6 @@
   </si>
   <si>
     <t>12345678</t>
-  </si>
-  <si>
-    <t>FOSS/GCMS Client ID</t>
   </si>
   <si>
     <t>[BUID:305939,RID:,ORP:4/5,DTS:2018-08-07 10:05:04][1] (Client) Unable to validate against database. / (Client) Impossible de valider dans la base de données.</t>
@@ -167,6 +164,48 @@
 iCARE - Immigration Contribution Agreement Reporting Environment
 Client Profile
 </t>
+  </si>
+  <si>
+    <t>dw</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>e232</t>
+  </si>
+  <si>
+    <t>3232</t>
+  </si>
+  <si>
+    <t>232</t>
+  </si>
+  <si>
+    <t>232332</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>r3rf3</t>
+  </si>
+  <si>
+    <t>ffefe</t>
+  </si>
+  <si>
+    <t>vevev</t>
+  </si>
+  <si>
+    <t>veve</t>
+  </si>
+  <si>
+    <t>vvve</t>
+  </si>
+  <si>
+    <t>vee</t>
+  </si>
+  <si>
+    <t>evev</t>
   </si>
 </sst>
 </file>
@@ -593,7 +632,7 @@
   <dimension ref="A1:Q2503"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15"/>
@@ -619,7 +658,7 @@
   <sheetData>
     <row r="1" spans="1:17" s="8" customFormat="1" ht="99.95" customHeight="1">
       <c r="A1" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -640,116 +679,116 @@
     </row>
     <row r="2" spans="1:17" hidden="1">
       <c r="A2" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="15.6" customHeight="1">
       <c r="A3" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N3" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Q3" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="126">
       <c r="A4" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>13</v>
+        <v>55</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>12</v>
@@ -757,7 +796,9 @@
       <c r="D4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="F4" s="2" t="s">
         <v>0</v>
       </c>
@@ -797,10 +838,18 @@
     </row>
     <row r="5" spans="1:17">
       <c r="A5" s="3"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+      <c r="B5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="F5" s="2"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -816,10 +865,18 @@
     </row>
     <row r="6" spans="1:17">
       <c r="A6" s="3"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+      <c r="B6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="F6" s="2"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -835,10 +892,18 @@
     </row>
     <row r="7" spans="1:17">
       <c r="A7" s="3"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+      <c r="B7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="F7" s="2"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -854,10 +919,18 @@
     </row>
     <row r="8" spans="1:17">
       <c r="A8" s="3"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="B8" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="F8" s="2"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>

</xml_diff>